<commit_message>
add: tempspeedup and tempspeeddown
Signed-off-by: trofimax <trofimenko@novomet.ru>
</commit_message>
<xml_diff>
--- a/documentation/registers.xlsx
+++ b/documentation/registers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4178" uniqueCount="2260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4196" uniqueCount="2267">
   <si>
     <t>Название</t>
   </si>
@@ -6796,6 +6796,27 @@
   </si>
   <si>
     <t>1.1 Текущие параметры ЧРП</t>
+  </si>
+  <si>
+    <t>VSD_TEMP_SPEEDUP</t>
+  </si>
+  <si>
+    <t>VSD_TEMP_SPEEDDOWN</t>
+  </si>
+  <si>
+    <t>Темп набора частоты</t>
+  </si>
+  <si>
+    <t>Темп снижения частоты</t>
+  </si>
+  <si>
+    <t>PHYSIC_TEMP</t>
+  </si>
+  <si>
+    <t>TEMP_HZ_SECOND</t>
+  </si>
+  <si>
+    <t>Гц/сек</t>
   </si>
 </sst>
 </file>
@@ -17272,11 +17293,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1097"/>
+  <dimension ref="A1:T1099"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A846" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E940" sqref="E940"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A847" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K880" sqref="K880"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38067,9 +38088,7 @@
       <c r="D647" s="14" t="s">
         <v>2082</v>
       </c>
-      <c r="E647" s="14" t="s">
-        <v>368</v>
-      </c>
+      <c r="E647" s="14"/>
       <c r="F647" s="14" t="s">
         <v>275</v>
       </c>
@@ -38120,9 +38139,7 @@
       <c r="D648" s="14" t="s">
         <v>2084</v>
       </c>
-      <c r="E648" s="14" t="s">
-        <v>368</v>
-      </c>
+      <c r="E648" s="14"/>
       <c r="F648" s="14" t="s">
         <v>275</v>
       </c>
@@ -44999,17 +45016,35 @@
         <v>10257</v>
       </c>
       <c r="B877" s="14" t="s">
-        <v>571</v>
-      </c>
-      <c r="C877" s="14"/>
-      <c r="D877" s="14"/>
-      <c r="E877" s="14"/>
-      <c r="F877" s="14"/>
-      <c r="G877" s="14"/>
-      <c r="H877" s="14"/>
-      <c r="I877" s="14"/>
-      <c r="J877" s="14"/>
-      <c r="K877" s="14"/>
+        <v>2260</v>
+      </c>
+      <c r="C877" s="14" t="s">
+        <v>2262</v>
+      </c>
+      <c r="D877" s="14" t="s">
+        <v>2262</v>
+      </c>
+      <c r="E877" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="F877" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G877" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H877" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="I877" s="14" t="s">
+        <v>2265</v>
+      </c>
+      <c r="J877" s="14" t="s">
+        <v>2266</v>
+      </c>
+      <c r="K877" s="14" t="s">
+        <v>276</v>
+      </c>
       <c r="L877" s="14"/>
       <c r="M877" s="14"/>
       <c r="N877" s="14"/>
@@ -45022,20 +45057,39 @@
     </row>
     <row r="878" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A878" s="14">
-        <v>15000</v>
+        <f t="shared" ref="A878:A879" si="19">A877+1</f>
+        <v>10258</v>
       </c>
       <c r="B878" s="14" t="s">
-        <v>1891</v>
-      </c>
-      <c r="C878" s="14"/>
-      <c r="D878" s="14"/>
-      <c r="E878" s="14"/>
-      <c r="F878" s="14"/>
-      <c r="G878" s="14"/>
-      <c r="H878" s="14"/>
-      <c r="I878" s="14"/>
-      <c r="J878" s="14"/>
-      <c r="K878" s="14"/>
+        <v>2261</v>
+      </c>
+      <c r="C878" s="14" t="s">
+        <v>2263</v>
+      </c>
+      <c r="D878" s="14" t="s">
+        <v>2263</v>
+      </c>
+      <c r="E878" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="F878" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G878" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H878" s="14" t="s">
+        <v>2264</v>
+      </c>
+      <c r="I878" s="14" t="s">
+        <v>2265</v>
+      </c>
+      <c r="J878" s="14" t="s">
+        <v>2266</v>
+      </c>
+      <c r="K878" s="14" t="s">
+        <v>276</v>
+      </c>
       <c r="L878" s="14"/>
       <c r="M878" s="14"/>
       <c r="N878" s="14"/>
@@ -45048,11 +45102,11 @@
     </row>
     <row r="879" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A879" s="14">
-        <f>A878+1</f>
-        <v>15001</v>
+        <f t="shared" si="19"/>
+        <v>10259</v>
       </c>
       <c r="B879" s="14" t="s">
-        <v>587</v>
+        <v>571</v>
       </c>
       <c r="C879" s="14"/>
       <c r="D879" s="14"/>
@@ -45070,46 +45124,25 @@
       <c r="P879" s="14"/>
       <c r="Q879" s="14"/>
       <c r="R879" s="14"/>
-      <c r="S879" s="14" t="s">
-        <v>1129</v>
-      </c>
+      <c r="S879" s="14"/>
       <c r="T879" s="14"/>
     </row>
     <row r="880" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A880" s="14">
-        <f t="shared" ref="A880:A935" si="19">A879+1</f>
-        <v>15002</v>
+        <v>15000</v>
       </c>
       <c r="B880" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="C880" s="14" t="s">
-        <v>1985</v>
-      </c>
-      <c r="D880" s="14" t="s">
-        <v>1986</v>
-      </c>
-      <c r="E880" s="14" t="s">
-        <v>2098</v>
-      </c>
-      <c r="F880" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G880" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H880" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="I880" s="14" t="s">
-        <v>1987</v>
-      </c>
-      <c r="J880" s="14" t="s">
-        <v>1988</v>
-      </c>
-      <c r="K880" s="14" t="s">
-        <v>299</v>
-      </c>
+        <v>1891</v>
+      </c>
+      <c r="C880" s="14"/>
+      <c r="D880" s="14"/>
+      <c r="E880" s="14"/>
+      <c r="F880" s="14"/>
+      <c r="G880" s="14"/>
+      <c r="H880" s="14"/>
+      <c r="I880" s="14"/>
+      <c r="J880" s="14"/>
+      <c r="K880" s="14"/>
       <c r="L880" s="14"/>
       <c r="M880" s="14"/>
       <c r="N880" s="14"/>
@@ -45117,46 +45150,26 @@
       <c r="P880" s="14"/>
       <c r="Q880" s="14"/>
       <c r="R880" s="14"/>
-      <c r="S880" s="14" t="s">
-        <v>1130</v>
-      </c>
+      <c r="S880" s="14"/>
       <c r="T880" s="14"/>
     </row>
     <row r="881" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A881" s="14">
-        <f t="shared" si="19"/>
-        <v>15003</v>
+        <f>A880+1</f>
+        <v>15001</v>
       </c>
       <c r="B881" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="C881" s="14" t="s">
-        <v>1989</v>
-      </c>
-      <c r="D881" s="14" t="s">
-        <v>1990</v>
-      </c>
-      <c r="E881" s="14" t="s">
-        <v>2098</v>
-      </c>
-      <c r="F881" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G881" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H881" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I881" s="14" t="s">
-        <v>548</v>
-      </c>
-      <c r="J881" s="14" t="s">
-        <v>1991</v>
-      </c>
-      <c r="K881" s="14" t="s">
-        <v>276</v>
-      </c>
+        <v>587</v>
+      </c>
+      <c r="C881" s="14"/>
+      <c r="D881" s="14"/>
+      <c r="E881" s="14"/>
+      <c r="F881" s="14"/>
+      <c r="G881" s="14"/>
+      <c r="H881" s="14"/>
+      <c r="I881" s="14"/>
+      <c r="J881" s="14"/>
+      <c r="K881" s="14"/>
       <c r="L881" s="14"/>
       <c r="M881" s="14"/>
       <c r="N881" s="14"/>
@@ -45165,25 +45178,27 @@
       <c r="Q881" s="14"/>
       <c r="R881" s="14"/>
       <c r="S881" s="14" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="T881" s="14"/>
     </row>
     <row r="882" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A882" s="14">
-        <f t="shared" si="19"/>
-        <v>15004</v>
+        <f t="shared" ref="A882:A937" si="20">A881+1</f>
+        <v>15002</v>
       </c>
       <c r="B882" s="14" t="s">
-        <v>614</v>
+        <v>296</v>
       </c>
       <c r="C882" s="14" t="s">
-        <v>1997</v>
+        <v>1985</v>
       </c>
       <c r="D882" s="14" t="s">
-        <v>1998</v>
-      </c>
-      <c r="E882" s="14"/>
+        <v>1986</v>
+      </c>
+      <c r="E882" s="14" t="s">
+        <v>2098</v>
+      </c>
       <c r="F882" s="14" t="s">
         <v>275</v>
       </c>
@@ -45191,16 +45206,16 @@
         <v>11</v>
       </c>
       <c r="H882" s="14" t="s">
-        <v>45</v>
+        <v>298</v>
       </c>
       <c r="I882" s="14" t="s">
-        <v>548</v>
+        <v>1987</v>
       </c>
       <c r="J882" s="14" t="s">
-        <v>1999</v>
+        <v>1988</v>
       </c>
       <c r="K882" s="14" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="L882" s="14"/>
       <c r="M882" s="14"/>
@@ -45210,27 +45225,45 @@
       <c r="Q882" s="14"/>
       <c r="R882" s="14"/>
       <c r="S882" s="14" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="T882" s="14"/>
     </row>
     <row r="883" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A883" s="14">
-        <f t="shared" si="19"/>
-        <v>15005</v>
+        <f t="shared" si="20"/>
+        <v>15003</v>
       </c>
       <c r="B883" s="14" t="s">
-        <v>615</v>
-      </c>
-      <c r="C883" s="14"/>
-      <c r="D883" s="14"/>
-      <c r="E883" s="14"/>
-      <c r="F883" s="14"/>
-      <c r="G883" s="14"/>
-      <c r="H883" s="14"/>
-      <c r="I883" s="14"/>
-      <c r="J883" s="14"/>
-      <c r="K883" s="14"/>
+        <v>300</v>
+      </c>
+      <c r="C883" s="14" t="s">
+        <v>1989</v>
+      </c>
+      <c r="D883" s="14" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E883" s="14" t="s">
+        <v>2098</v>
+      </c>
+      <c r="F883" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G883" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H883" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I883" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="J883" s="14" t="s">
+        <v>1991</v>
+      </c>
+      <c r="K883" s="14" t="s">
+        <v>276</v>
+      </c>
       <c r="L883" s="14"/>
       <c r="M883" s="14"/>
       <c r="N883" s="14"/>
@@ -45239,27 +45272,43 @@
       <c r="Q883" s="14"/>
       <c r="R883" s="14"/>
       <c r="S883" s="14" t="s">
-        <v>2110</v>
+        <v>1131</v>
       </c>
       <c r="T883" s="14"/>
     </row>
     <row r="884" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A884" s="14">
-        <f t="shared" si="19"/>
-        <v>15006</v>
+        <f t="shared" si="20"/>
+        <v>15004</v>
       </c>
       <c r="B884" s="14" t="s">
-        <v>616</v>
-      </c>
-      <c r="C884" s="14"/>
-      <c r="D884" s="14"/>
+        <v>614</v>
+      </c>
+      <c r="C884" s="14" t="s">
+        <v>1997</v>
+      </c>
+      <c r="D884" s="14" t="s">
+        <v>1998</v>
+      </c>
       <c r="E884" s="14"/>
-      <c r="F884" s="14"/>
-      <c r="G884" s="14"/>
-      <c r="H884" s="14"/>
-      <c r="I884" s="14"/>
-      <c r="J884" s="14"/>
-      <c r="K884" s="14"/>
+      <c r="F884" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G884" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H884" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I884" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="J884" s="14" t="s">
+        <v>1999</v>
+      </c>
+      <c r="K884" s="14" t="s">
+        <v>276</v>
+      </c>
       <c r="L884" s="14"/>
       <c r="M884" s="14"/>
       <c r="N884" s="14"/>
@@ -45268,45 +45317,27 @@
       <c r="Q884" s="14"/>
       <c r="R884" s="14"/>
       <c r="S884" s="14" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="T884" s="14"/>
     </row>
     <row r="885" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A885" s="14">
-        <f t="shared" si="19"/>
-        <v>15007</v>
+        <f t="shared" si="20"/>
+        <v>15005</v>
       </c>
       <c r="B885" s="14" t="s">
-        <v>617</v>
-      </c>
-      <c r="C885" s="14" t="s">
-        <v>1996</v>
-      </c>
-      <c r="D885" s="14" t="s">
-        <v>1995</v>
-      </c>
-      <c r="E885" s="14" t="s">
-        <v>2099</v>
-      </c>
-      <c r="F885" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G885" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H885" s="14" t="s">
-        <v>1992</v>
-      </c>
-      <c r="I885" s="14" t="s">
-        <v>1993</v>
-      </c>
-      <c r="J885" s="14" t="s">
-        <v>1994</v>
-      </c>
-      <c r="K885" s="14" t="s">
-        <v>299</v>
-      </c>
+        <v>615</v>
+      </c>
+      <c r="C885" s="14"/>
+      <c r="D885" s="14"/>
+      <c r="E885" s="14"/>
+      <c r="F885" s="14"/>
+      <c r="G885" s="14"/>
+      <c r="H885" s="14"/>
+      <c r="I885" s="14"/>
+      <c r="J885" s="14"/>
+      <c r="K885" s="14"/>
       <c r="L885" s="14"/>
       <c r="M885" s="14"/>
       <c r="N885" s="14"/>
@@ -45315,45 +45346,27 @@
       <c r="Q885" s="14"/>
       <c r="R885" s="14"/>
       <c r="S885" s="14" t="s">
-        <v>1134</v>
+        <v>2110</v>
       </c>
       <c r="T885" s="14"/>
     </row>
     <row r="886" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A886" s="14">
-        <f t="shared" si="19"/>
-        <v>15008</v>
+        <f t="shared" si="20"/>
+        <v>15006</v>
       </c>
       <c r="B886" s="14" t="s">
-        <v>618</v>
-      </c>
-      <c r="C886" s="14" t="s">
-        <v>2000</v>
-      </c>
-      <c r="D886" s="14" t="s">
-        <v>2001</v>
-      </c>
-      <c r="E886" s="14" t="s">
-        <v>2099</v>
-      </c>
-      <c r="F886" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G886" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H886" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="I886" s="14" t="s">
-        <v>1987</v>
-      </c>
-      <c r="J886" s="14" t="s">
-        <v>1988</v>
-      </c>
-      <c r="K886" s="14" t="s">
-        <v>299</v>
-      </c>
+        <v>616</v>
+      </c>
+      <c r="C886" s="14"/>
+      <c r="D886" s="14"/>
+      <c r="E886" s="14"/>
+      <c r="F886" s="14"/>
+      <c r="G886" s="14"/>
+      <c r="H886" s="14"/>
+      <c r="I886" s="14"/>
+      <c r="J886" s="14"/>
+      <c r="K886" s="14"/>
       <c r="L886" s="14"/>
       <c r="M886" s="14"/>
       <c r="N886" s="14"/>
@@ -45362,23 +45375,23 @@
       <c r="Q886" s="14"/>
       <c r="R886" s="14"/>
       <c r="S886" s="14" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="T886" s="14"/>
     </row>
     <row r="887" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A887" s="14">
-        <f t="shared" si="19"/>
-        <v>15009</v>
+        <f t="shared" si="20"/>
+        <v>15007</v>
       </c>
       <c r="B887" s="14" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C887" s="14" t="s">
-        <v>2002</v>
+        <v>1996</v>
       </c>
       <c r="D887" s="14" t="s">
-        <v>2003</v>
+        <v>1995</v>
       </c>
       <c r="E887" s="14" t="s">
         <v>2099</v>
@@ -45390,16 +45403,16 @@
         <v>11</v>
       </c>
       <c r="H887" s="14" t="s">
-        <v>45</v>
+        <v>1992</v>
       </c>
       <c r="I887" s="14" t="s">
-        <v>548</v>
+        <v>1993</v>
       </c>
       <c r="J887" s="14" t="s">
-        <v>1999</v>
+        <v>1994</v>
       </c>
       <c r="K887" s="14" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="L887" s="14"/>
       <c r="M887" s="14"/>
@@ -45409,23 +45422,23 @@
       <c r="Q887" s="14"/>
       <c r="R887" s="14"/>
       <c r="S887" s="14" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="T887" s="14"/>
     </row>
     <row r="888" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A888" s="14">
-        <f t="shared" si="19"/>
-        <v>15010</v>
+        <f t="shared" si="20"/>
+        <v>15008</v>
       </c>
       <c r="B888" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C888" s="14" t="s">
-        <v>2004</v>
+        <v>2000</v>
       </c>
       <c r="D888" s="14" t="s">
-        <v>2005</v>
+        <v>2001</v>
       </c>
       <c r="E888" s="14" t="s">
         <v>2099</v>
@@ -45437,16 +45450,16 @@
         <v>11</v>
       </c>
       <c r="H888" s="14" t="s">
-        <v>2006</v>
+        <v>298</v>
       </c>
       <c r="I888" s="14" t="s">
-        <v>2007</v>
+        <v>1987</v>
       </c>
       <c r="J888" s="14" t="s">
-        <v>2008</v>
+        <v>1988</v>
       </c>
       <c r="K888" s="14" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="L888" s="14"/>
       <c r="M888" s="14"/>
@@ -45456,23 +45469,23 @@
       <c r="Q888" s="14"/>
       <c r="R888" s="14"/>
       <c r="S888" s="14" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="T888" s="14"/>
     </row>
     <row r="889" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A889" s="14">
-        <f t="shared" si="19"/>
-        <v>15011</v>
+        <f t="shared" si="20"/>
+        <v>15009</v>
       </c>
       <c r="B889" s="14" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C889" s="14" t="s">
-        <v>2111</v>
+        <v>2002</v>
       </c>
       <c r="D889" s="14" t="s">
-        <v>2112</v>
+        <v>2003</v>
       </c>
       <c r="E889" s="14" t="s">
         <v>2099</v>
@@ -45484,16 +45497,16 @@
         <v>11</v>
       </c>
       <c r="H889" s="14" t="s">
-        <v>1992</v>
+        <v>45</v>
       </c>
       <c r="I889" s="14" t="s">
-        <v>1993</v>
+        <v>548</v>
       </c>
       <c r="J889" s="14" t="s">
-        <v>1994</v>
+        <v>1999</v>
       </c>
       <c r="K889" s="14" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="L889" s="14"/>
       <c r="M889" s="14"/>
@@ -45503,27 +45516,45 @@
       <c r="Q889" s="14"/>
       <c r="R889" s="14"/>
       <c r="S889" s="14" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="T889" s="14"/>
     </row>
     <row r="890" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A890" s="14">
-        <f t="shared" si="19"/>
-        <v>15012</v>
+        <f t="shared" si="20"/>
+        <v>15010</v>
       </c>
       <c r="B890" s="14" t="s">
-        <v>622</v>
-      </c>
-      <c r="C890" s="14"/>
-      <c r="D890" s="14"/>
-      <c r="E890" s="14"/>
-      <c r="F890" s="14"/>
-      <c r="G890" s="14"/>
-      <c r="H890" s="14"/>
-      <c r="I890" s="14"/>
-      <c r="J890" s="14"/>
-      <c r="K890" s="14"/>
+        <v>620</v>
+      </c>
+      <c r="C890" s="14" t="s">
+        <v>2004</v>
+      </c>
+      <c r="D890" s="14" t="s">
+        <v>2005</v>
+      </c>
+      <c r="E890" s="14" t="s">
+        <v>2099</v>
+      </c>
+      <c r="F890" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G890" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H890" s="14" t="s">
+        <v>2006</v>
+      </c>
+      <c r="I890" s="14" t="s">
+        <v>2007</v>
+      </c>
+      <c r="J890" s="14" t="s">
+        <v>2008</v>
+      </c>
+      <c r="K890" s="14" t="s">
+        <v>286</v>
+      </c>
       <c r="L890" s="14"/>
       <c r="M890" s="14"/>
       <c r="N890" s="14"/>
@@ -45532,27 +45563,45 @@
       <c r="Q890" s="14"/>
       <c r="R890" s="14"/>
       <c r="S890" s="14" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="T890" s="14"/>
     </row>
     <row r="891" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A891" s="14">
-        <f t="shared" si="19"/>
-        <v>15013</v>
+        <f t="shared" si="20"/>
+        <v>15011</v>
       </c>
       <c r="B891" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="C891" s="14"/>
-      <c r="D891" s="14"/>
-      <c r="E891" s="14"/>
-      <c r="F891" s="14"/>
-      <c r="G891" s="14"/>
-      <c r="H891" s="14"/>
-      <c r="I891" s="14"/>
-      <c r="J891" s="14"/>
-      <c r="K891" s="14"/>
+        <v>621</v>
+      </c>
+      <c r="C891" s="14" t="s">
+        <v>2111</v>
+      </c>
+      <c r="D891" s="14" t="s">
+        <v>2112</v>
+      </c>
+      <c r="E891" s="14" t="s">
+        <v>2099</v>
+      </c>
+      <c r="F891" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G891" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H891" s="14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="I891" s="14" t="s">
+        <v>1993</v>
+      </c>
+      <c r="J891" s="14" t="s">
+        <v>1994</v>
+      </c>
+      <c r="K891" s="14" t="s">
+        <v>299</v>
+      </c>
       <c r="L891" s="14"/>
       <c r="M891" s="14"/>
       <c r="N891" s="14"/>
@@ -45561,17 +45610,17 @@
       <c r="Q891" s="14"/>
       <c r="R891" s="14"/>
       <c r="S891" s="14" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
       <c r="T891" s="14"/>
     </row>
     <row r="892" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A892" s="14">
-        <f t="shared" si="19"/>
-        <v>15014</v>
+        <f t="shared" si="20"/>
+        <v>15012</v>
       </c>
       <c r="B892" s="14" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C892" s="14"/>
       <c r="D892" s="14"/>
@@ -45590,17 +45639,17 @@
       <c r="Q892" s="14"/>
       <c r="R892" s="14"/>
       <c r="S892" s="14" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="T892" s="14"/>
     </row>
     <row r="893" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A893" s="14">
-        <f t="shared" si="19"/>
-        <v>15015</v>
+        <f t="shared" si="20"/>
+        <v>15013</v>
       </c>
       <c r="B893" s="14" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C893" s="14"/>
       <c r="D893" s="14"/>
@@ -45619,17 +45668,17 @@
       <c r="Q893" s="14"/>
       <c r="R893" s="14"/>
       <c r="S893" s="14" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="T893" s="14"/>
     </row>
     <row r="894" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A894" s="14">
-        <f t="shared" si="19"/>
-        <v>15016</v>
+        <f t="shared" si="20"/>
+        <v>15014</v>
       </c>
       <c r="B894" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C894" s="14"/>
       <c r="D894" s="14"/>
@@ -45648,17 +45697,17 @@
       <c r="Q894" s="14"/>
       <c r="R894" s="14"/>
       <c r="S894" s="14" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="T894" s="14"/>
     </row>
     <row r="895" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A895" s="14">
-        <f t="shared" si="19"/>
-        <v>15017</v>
+        <f t="shared" si="20"/>
+        <v>15015</v>
       </c>
       <c r="B895" s="14" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C895" s="14"/>
       <c r="D895" s="14"/>
@@ -45677,17 +45726,17 @@
       <c r="Q895" s="14"/>
       <c r="R895" s="14"/>
       <c r="S895" s="14" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="T895" s="14"/>
     </row>
     <row r="896" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A896" s="14">
-        <f t="shared" si="19"/>
-        <v>15018</v>
+        <f t="shared" si="20"/>
+        <v>15016</v>
       </c>
       <c r="B896" s="14" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C896" s="14"/>
       <c r="D896" s="14"/>
@@ -45706,17 +45755,17 @@
       <c r="Q896" s="14"/>
       <c r="R896" s="14"/>
       <c r="S896" s="14" t="s">
-        <v>666</v>
+        <v>1142</v>
       </c>
       <c r="T896" s="14"/>
     </row>
     <row r="897" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A897" s="14">
-        <f t="shared" si="19"/>
-        <v>15019</v>
+        <f t="shared" si="20"/>
+        <v>15017</v>
       </c>
       <c r="B897" s="14" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C897" s="14"/>
       <c r="D897" s="14"/>
@@ -45735,17 +45784,17 @@
       <c r="Q897" s="14"/>
       <c r="R897" s="14"/>
       <c r="S897" s="14" t="s">
-        <v>667</v>
+        <v>1143</v>
       </c>
       <c r="T897" s="14"/>
     </row>
     <row r="898" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A898" s="14">
-        <f t="shared" si="19"/>
-        <v>15020</v>
+        <f t="shared" si="20"/>
+        <v>15018</v>
       </c>
       <c r="B898" s="14" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C898" s="14"/>
       <c r="D898" s="14"/>
@@ -45764,17 +45813,17 @@
       <c r="Q898" s="14"/>
       <c r="R898" s="14"/>
       <c r="S898" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="T898" s="14"/>
     </row>
     <row r="899" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A899" s="14">
-        <f t="shared" si="19"/>
-        <v>15021</v>
+        <f t="shared" si="20"/>
+        <v>15019</v>
       </c>
       <c r="B899" s="14" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C899" s="14"/>
       <c r="D899" s="14"/>
@@ -45793,17 +45842,17 @@
       <c r="Q899" s="14"/>
       <c r="R899" s="14"/>
       <c r="S899" s="14" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="T899" s="14"/>
     </row>
     <row r="900" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A900" s="14">
-        <f t="shared" si="19"/>
-        <v>15022</v>
+        <f t="shared" si="20"/>
+        <v>15020</v>
       </c>
       <c r="B900" s="14" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C900" s="14"/>
       <c r="D900" s="14"/>
@@ -45822,17 +45871,17 @@
       <c r="Q900" s="14"/>
       <c r="R900" s="14"/>
       <c r="S900" s="14" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="T900" s="14"/>
     </row>
     <row r="901" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A901" s="14">
-        <f t="shared" si="19"/>
-        <v>15023</v>
+        <f t="shared" si="20"/>
+        <v>15021</v>
       </c>
       <c r="B901" s="14" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C901" s="14"/>
       <c r="D901" s="14"/>
@@ -45851,17 +45900,17 @@
       <c r="Q901" s="14"/>
       <c r="R901" s="14"/>
       <c r="S901" s="14" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="T901" s="14"/>
     </row>
     <row r="902" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A902" s="14">
-        <f t="shared" si="19"/>
-        <v>15024</v>
+        <f t="shared" si="20"/>
+        <v>15022</v>
       </c>
       <c r="B902" s="14" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C902" s="14"/>
       <c r="D902" s="14"/>
@@ -45880,17 +45929,17 @@
       <c r="Q902" s="14"/>
       <c r="R902" s="14"/>
       <c r="S902" s="14" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="T902" s="14"/>
     </row>
     <row r="903" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A903" s="14">
-        <f t="shared" si="19"/>
-        <v>15025</v>
+        <f t="shared" si="20"/>
+        <v>15023</v>
       </c>
       <c r="B903" s="14" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C903" s="14"/>
       <c r="D903" s="14"/>
@@ -45909,17 +45958,17 @@
       <c r="Q903" s="14"/>
       <c r="R903" s="14"/>
       <c r="S903" s="14" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="T903" s="14"/>
     </row>
     <row r="904" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A904" s="14">
-        <f t="shared" si="19"/>
-        <v>15026</v>
+        <f t="shared" si="20"/>
+        <v>15024</v>
       </c>
       <c r="B904" s="14" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C904" s="14"/>
       <c r="D904" s="14"/>
@@ -45938,17 +45987,17 @@
       <c r="Q904" s="14"/>
       <c r="R904" s="14"/>
       <c r="S904" s="14" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="T904" s="14"/>
     </row>
     <row r="905" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A905" s="14">
-        <f t="shared" si="19"/>
-        <v>15027</v>
+        <f t="shared" si="20"/>
+        <v>15025</v>
       </c>
       <c r="B905" s="14" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C905" s="14"/>
       <c r="D905" s="14"/>
@@ -45967,17 +46016,17 @@
       <c r="Q905" s="14"/>
       <c r="R905" s="14"/>
       <c r="S905" s="14" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="T905" s="14"/>
     </row>
     <row r="906" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A906" s="14">
-        <f t="shared" si="19"/>
-        <v>15028</v>
+        <f t="shared" si="20"/>
+        <v>15026</v>
       </c>
       <c r="B906" s="14" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C906" s="14"/>
       <c r="D906" s="14"/>
@@ -45996,17 +46045,17 @@
       <c r="Q906" s="14"/>
       <c r="R906" s="14"/>
       <c r="S906" s="14" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="T906" s="14"/>
     </row>
     <row r="907" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A907" s="14">
-        <f t="shared" si="19"/>
-        <v>15029</v>
+        <f t="shared" si="20"/>
+        <v>15027</v>
       </c>
       <c r="B907" s="14" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C907" s="14"/>
       <c r="D907" s="14"/>
@@ -46025,17 +46074,17 @@
       <c r="Q907" s="14"/>
       <c r="R907" s="14"/>
       <c r="S907" s="14" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="T907" s="14"/>
     </row>
     <row r="908" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A908" s="14">
-        <f t="shared" si="19"/>
-        <v>15030</v>
+        <f t="shared" si="20"/>
+        <v>15028</v>
       </c>
       <c r="B908" s="14" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C908" s="14"/>
       <c r="D908" s="14"/>
@@ -46054,17 +46103,17 @@
       <c r="Q908" s="14"/>
       <c r="R908" s="14"/>
       <c r="S908" s="14" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="T908" s="14"/>
     </row>
     <row r="909" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A909" s="14">
-        <f t="shared" si="19"/>
-        <v>15031</v>
+        <f t="shared" si="20"/>
+        <v>15029</v>
       </c>
       <c r="B909" s="14" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C909" s="14"/>
       <c r="D909" s="14"/>
@@ -46083,17 +46132,17 @@
       <c r="Q909" s="14"/>
       <c r="R909" s="14"/>
       <c r="S909" s="14" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="T909" s="14"/>
     </row>
     <row r="910" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A910" s="14">
-        <f t="shared" si="19"/>
-        <v>15032</v>
+        <f t="shared" si="20"/>
+        <v>15030</v>
       </c>
       <c r="B910" s="14" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C910" s="14"/>
       <c r="D910" s="14"/>
@@ -46112,17 +46161,17 @@
       <c r="Q910" s="14"/>
       <c r="R910" s="14"/>
       <c r="S910" s="14" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="T910" s="14"/>
     </row>
     <row r="911" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A911" s="14">
-        <f t="shared" si="19"/>
-        <v>15033</v>
+        <f t="shared" si="20"/>
+        <v>15031</v>
       </c>
       <c r="B911" s="14" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C911" s="14"/>
       <c r="D911" s="14"/>
@@ -46141,17 +46190,17 @@
       <c r="Q911" s="14"/>
       <c r="R911" s="14"/>
       <c r="S911" s="14" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="T911" s="14"/>
     </row>
     <row r="912" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A912" s="14">
-        <f t="shared" si="19"/>
-        <v>15034</v>
+        <f t="shared" si="20"/>
+        <v>15032</v>
       </c>
       <c r="B912" s="14" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C912" s="14"/>
       <c r="D912" s="14"/>
@@ -46170,17 +46219,17 @@
       <c r="Q912" s="14"/>
       <c r="R912" s="14"/>
       <c r="S912" s="14" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="T912" s="14"/>
     </row>
     <row r="913" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A913" s="14">
-        <f t="shared" si="19"/>
-        <v>15035</v>
+        <f t="shared" si="20"/>
+        <v>15033</v>
       </c>
       <c r="B913" s="14" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C913" s="14"/>
       <c r="D913" s="14"/>
@@ -46199,17 +46248,17 @@
       <c r="Q913" s="14"/>
       <c r="R913" s="14"/>
       <c r="S913" s="14" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="T913" s="14"/>
     </row>
     <row r="914" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A914" s="14">
-        <f t="shared" si="19"/>
-        <v>15036</v>
+        <f t="shared" si="20"/>
+        <v>15034</v>
       </c>
       <c r="B914" s="14" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C914" s="14"/>
       <c r="D914" s="14"/>
@@ -46228,17 +46277,17 @@
       <c r="Q914" s="14"/>
       <c r="R914" s="14"/>
       <c r="S914" s="14" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="T914" s="14"/>
     </row>
     <row r="915" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A915" s="14">
-        <f t="shared" si="19"/>
-        <v>15037</v>
+        <f t="shared" si="20"/>
+        <v>15035</v>
       </c>
       <c r="B915" s="14" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C915" s="14"/>
       <c r="D915" s="14"/>
@@ -46257,17 +46306,17 @@
       <c r="Q915" s="14"/>
       <c r="R915" s="14"/>
       <c r="S915" s="14" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="T915" s="14"/>
     </row>
     <row r="916" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A916" s="14">
-        <f t="shared" si="19"/>
-        <v>15038</v>
+        <f t="shared" si="20"/>
+        <v>15036</v>
       </c>
       <c r="B916" s="14" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C916" s="14"/>
       <c r="D916" s="14"/>
@@ -46286,17 +46335,17 @@
       <c r="Q916" s="14"/>
       <c r="R916" s="14"/>
       <c r="S916" s="14" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="T916" s="14"/>
     </row>
     <row r="917" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A917" s="14">
-        <f t="shared" si="19"/>
-        <v>15039</v>
+        <f t="shared" si="20"/>
+        <v>15037</v>
       </c>
       <c r="B917" s="14" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C917" s="14"/>
       <c r="D917" s="14"/>
@@ -46315,17 +46364,17 @@
       <c r="Q917" s="14"/>
       <c r="R917" s="14"/>
       <c r="S917" s="14" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="T917" s="14"/>
     </row>
     <row r="918" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A918" s="14">
-        <f t="shared" si="19"/>
-        <v>15040</v>
+        <f t="shared" si="20"/>
+        <v>15038</v>
       </c>
       <c r="B918" s="14" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C918" s="14"/>
       <c r="D918" s="14"/>
@@ -46344,17 +46393,17 @@
       <c r="Q918" s="14"/>
       <c r="R918" s="14"/>
       <c r="S918" s="14" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="T918" s="14"/>
     </row>
     <row r="919" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A919" s="14">
-        <f t="shared" si="19"/>
-        <v>15041</v>
+        <f t="shared" si="20"/>
+        <v>15039</v>
       </c>
       <c r="B919" s="14" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C919" s="14"/>
       <c r="D919" s="14"/>
@@ -46373,17 +46422,17 @@
       <c r="Q919" s="14"/>
       <c r="R919" s="14"/>
       <c r="S919" s="14" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="T919" s="14"/>
     </row>
     <row r="920" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A920" s="14">
-        <f t="shared" si="19"/>
-        <v>15042</v>
+        <f t="shared" si="20"/>
+        <v>15040</v>
       </c>
       <c r="B920" s="14" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C920" s="14"/>
       <c r="D920" s="14"/>
@@ -46402,17 +46451,17 @@
       <c r="Q920" s="14"/>
       <c r="R920" s="14"/>
       <c r="S920" s="14" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="T920" s="14"/>
     </row>
     <row r="921" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A921" s="14">
-        <f t="shared" si="19"/>
-        <v>15043</v>
+        <f t="shared" si="20"/>
+        <v>15041</v>
       </c>
       <c r="B921" s="14" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C921" s="14"/>
       <c r="D921" s="14"/>
@@ -46431,17 +46480,17 @@
       <c r="Q921" s="14"/>
       <c r="R921" s="14"/>
       <c r="S921" s="14" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="T921" s="14"/>
     </row>
     <row r="922" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A922" s="14">
-        <f t="shared" si="19"/>
-        <v>15044</v>
+        <f t="shared" si="20"/>
+        <v>15042</v>
       </c>
       <c r="B922" s="14" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C922" s="14"/>
       <c r="D922" s="14"/>
@@ -46460,17 +46509,17 @@
       <c r="Q922" s="14"/>
       <c r="R922" s="14"/>
       <c r="S922" s="14" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="T922" s="14"/>
     </row>
     <row r="923" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A923" s="14">
-        <f t="shared" si="19"/>
-        <v>15045</v>
+        <f t="shared" si="20"/>
+        <v>15043</v>
       </c>
       <c r="B923" s="14" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C923" s="14"/>
       <c r="D923" s="14"/>
@@ -46489,17 +46538,17 @@
       <c r="Q923" s="14"/>
       <c r="R923" s="14"/>
       <c r="S923" s="14" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="T923" s="14"/>
     </row>
     <row r="924" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A924" s="14">
-        <f t="shared" si="19"/>
-        <v>15046</v>
+        <f t="shared" si="20"/>
+        <v>15044</v>
       </c>
       <c r="B924" s="14" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C924" s="14"/>
       <c r="D924" s="14"/>
@@ -46518,17 +46567,17 @@
       <c r="Q924" s="14"/>
       <c r="R924" s="14"/>
       <c r="S924" s="14" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="T924" s="14"/>
     </row>
     <row r="925" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A925" s="14">
-        <f t="shared" si="19"/>
-        <v>15047</v>
+        <f t="shared" si="20"/>
+        <v>15045</v>
       </c>
       <c r="B925" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C925" s="14"/>
       <c r="D925" s="14"/>
@@ -46547,17 +46596,17 @@
       <c r="Q925" s="14"/>
       <c r="R925" s="14"/>
       <c r="S925" s="14" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="T925" s="14"/>
     </row>
     <row r="926" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A926" s="14">
-        <f t="shared" si="19"/>
-        <v>15048</v>
+        <f t="shared" si="20"/>
+        <v>15046</v>
       </c>
       <c r="B926" s="14" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C926" s="14"/>
       <c r="D926" s="14"/>
@@ -46576,17 +46625,17 @@
       <c r="Q926" s="14"/>
       <c r="R926" s="14"/>
       <c r="S926" s="14" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="T926" s="14"/>
     </row>
     <row r="927" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A927" s="14">
-        <f t="shared" si="19"/>
-        <v>15049</v>
+        <f t="shared" si="20"/>
+        <v>15047</v>
       </c>
       <c r="B927" s="14" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C927" s="14"/>
       <c r="D927" s="14"/>
@@ -46605,17 +46654,17 @@
       <c r="Q927" s="14"/>
       <c r="R927" s="14"/>
       <c r="S927" s="14" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="T927" s="14"/>
     </row>
     <row r="928" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A928" s="14">
-        <f t="shared" si="19"/>
-        <v>15050</v>
+        <f t="shared" si="20"/>
+        <v>15048</v>
       </c>
       <c r="B928" s="14" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C928" s="14"/>
       <c r="D928" s="14"/>
@@ -46634,17 +46683,17 @@
       <c r="Q928" s="14"/>
       <c r="R928" s="14"/>
       <c r="S928" s="14" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="T928" s="14"/>
     </row>
     <row r="929" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A929" s="14">
-        <f t="shared" si="19"/>
-        <v>15051</v>
+        <f t="shared" si="20"/>
+        <v>15049</v>
       </c>
       <c r="B929" s="14" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C929" s="14"/>
       <c r="D929" s="14"/>
@@ -46663,17 +46712,17 @@
       <c r="Q929" s="14"/>
       <c r="R929" s="14"/>
       <c r="S929" s="14" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="T929" s="14"/>
     </row>
     <row r="930" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A930" s="14">
-        <f t="shared" si="19"/>
-        <v>15052</v>
+        <f t="shared" si="20"/>
+        <v>15050</v>
       </c>
       <c r="B930" s="14" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C930" s="14"/>
       <c r="D930" s="14"/>
@@ -46692,17 +46741,17 @@
       <c r="Q930" s="14"/>
       <c r="R930" s="14"/>
       <c r="S930" s="14" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="T930" s="14"/>
     </row>
     <row r="931" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A931" s="14">
-        <f t="shared" si="19"/>
-        <v>15053</v>
+        <f t="shared" si="20"/>
+        <v>15051</v>
       </c>
       <c r="B931" s="14" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C931" s="14"/>
       <c r="D931" s="14"/>
@@ -46721,17 +46770,17 @@
       <c r="Q931" s="14"/>
       <c r="R931" s="14"/>
       <c r="S931" s="14" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="T931" s="14"/>
     </row>
     <row r="932" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A932" s="14">
-        <f t="shared" si="19"/>
-        <v>15054</v>
+        <f t="shared" si="20"/>
+        <v>15052</v>
       </c>
       <c r="B932" s="14" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C932" s="14"/>
       <c r="D932" s="14"/>
@@ -46750,17 +46799,17 @@
       <c r="Q932" s="14"/>
       <c r="R932" s="14"/>
       <c r="S932" s="14" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="T932" s="14"/>
     </row>
     <row r="933" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A933" s="14">
-        <f t="shared" si="19"/>
-        <v>15055</v>
+        <f t="shared" si="20"/>
+        <v>15053</v>
       </c>
       <c r="B933" s="14" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C933" s="14"/>
       <c r="D933" s="14"/>
@@ -46779,17 +46828,17 @@
       <c r="Q933" s="14"/>
       <c r="R933" s="14"/>
       <c r="S933" s="14" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="T933" s="14"/>
     </row>
     <row r="934" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A934" s="14">
-        <f t="shared" si="19"/>
-        <v>15056</v>
+        <f t="shared" si="20"/>
+        <v>15054</v>
       </c>
       <c r="B934" s="14" t="s">
-        <v>704</v>
+        <v>664</v>
       </c>
       <c r="C934" s="14"/>
       <c r="D934" s="14"/>
@@ -46808,17 +46857,17 @@
       <c r="Q934" s="14"/>
       <c r="R934" s="14"/>
       <c r="S934" s="14" t="s">
-        <v>1144</v>
+        <v>702</v>
       </c>
       <c r="T934" s="14"/>
     </row>
     <row r="935" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A935" s="14">
-        <f t="shared" si="19"/>
-        <v>15057</v>
+        <f t="shared" si="20"/>
+        <v>15055</v>
       </c>
       <c r="B935" s="14" t="s">
-        <v>597</v>
+        <v>665</v>
       </c>
       <c r="C935" s="14"/>
       <c r="D935" s="14"/>
@@ -46836,15 +46885,18 @@
       <c r="P935" s="14"/>
       <c r="Q935" s="14"/>
       <c r="R935" s="14"/>
-      <c r="S935" s="14"/>
+      <c r="S935" s="14" t="s">
+        <v>703</v>
+      </c>
       <c r="T935" s="14"/>
     </row>
     <row r="936" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A936" s="14">
-        <v>20000</v>
+        <f t="shared" si="20"/>
+        <v>15056</v>
       </c>
       <c r="B936" s="14" t="s">
-        <v>1892</v>
+        <v>704</v>
       </c>
       <c r="C936" s="14"/>
       <c r="D936" s="14"/>
@@ -46863,45 +46915,27 @@
       <c r="Q936" s="14"/>
       <c r="R936" s="14"/>
       <c r="S936" s="14" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="T936" s="14"/>
     </row>
     <row r="937" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A937" s="14">
-        <f>A936+1</f>
-        <v>20001</v>
+        <f t="shared" si="20"/>
+        <v>15057</v>
       </c>
       <c r="B937" s="14" t="s">
-        <v>599</v>
-      </c>
-      <c r="C937" s="14" t="s">
-        <v>1968</v>
-      </c>
-      <c r="D937" s="14" t="s">
-        <v>1971</v>
-      </c>
-      <c r="E937" s="14" t="s">
-        <v>2090</v>
-      </c>
-      <c r="F937" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G937" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H937" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I937" s="14" t="s">
-        <v>547</v>
-      </c>
-      <c r="J937" s="14" t="s">
-        <v>1964</v>
-      </c>
-      <c r="K937" s="14" t="s">
-        <v>1947</v>
-      </c>
+        <v>597</v>
+      </c>
+      <c r="C937" s="14"/>
+      <c r="D937" s="14"/>
+      <c r="E937" s="14"/>
+      <c r="F937" s="14"/>
+      <c r="G937" s="14"/>
+      <c r="H937" s="14"/>
+      <c r="I937" s="14"/>
+      <c r="J937" s="14"/>
+      <c r="K937" s="14"/>
       <c r="L937" s="14"/>
       <c r="M937" s="14"/>
       <c r="N937" s="14"/>
@@ -46909,46 +46943,25 @@
       <c r="P937" s="14"/>
       <c r="Q937" s="14"/>
       <c r="R937" s="14"/>
-      <c r="S937" s="14" t="s">
-        <v>1146</v>
-      </c>
+      <c r="S937" s="14"/>
       <c r="T937" s="14"/>
     </row>
     <row r="938" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A938" s="14">
-        <f t="shared" ref="A938:A987" si="20">A937+1</f>
-        <v>20002</v>
+        <v>20000</v>
       </c>
       <c r="B938" s="14" t="s">
-        <v>600</v>
-      </c>
-      <c r="C938" s="14" t="s">
-        <v>1969</v>
-      </c>
-      <c r="D938" s="14" t="s">
-        <v>1972</v>
-      </c>
-      <c r="E938" s="14" t="s">
-        <v>2090</v>
-      </c>
-      <c r="F938" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G938" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H938" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I938" s="14" t="s">
-        <v>547</v>
-      </c>
-      <c r="J938" s="14" t="s">
-        <v>1964</v>
-      </c>
-      <c r="K938" s="14" t="s">
-        <v>1947</v>
-      </c>
+        <v>1892</v>
+      </c>
+      <c r="C938" s="14"/>
+      <c r="D938" s="14"/>
+      <c r="E938" s="14"/>
+      <c r="F938" s="14"/>
+      <c r="G938" s="14"/>
+      <c r="H938" s="14"/>
+      <c r="I938" s="14"/>
+      <c r="J938" s="14"/>
+      <c r="K938" s="14"/>
       <c r="L938" s="14"/>
       <c r="M938" s="14"/>
       <c r="N938" s="14"/>
@@ -46957,23 +46970,23 @@
       <c r="Q938" s="14"/>
       <c r="R938" s="14"/>
       <c r="S938" s="14" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="T938" s="14"/>
     </row>
     <row r="939" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A939" s="14">
-        <f t="shared" si="20"/>
-        <v>20003</v>
+        <f>A938+1</f>
+        <v>20001</v>
       </c>
       <c r="B939" s="14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C939" s="14" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="D939" s="14" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="E939" s="14" t="s">
         <v>2090</v>
@@ -47004,33 +47017,45 @@
       <c r="Q939" s="14"/>
       <c r="R939" s="14"/>
       <c r="S939" s="14" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="T939" s="14"/>
     </row>
     <row r="940" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A940" s="14">
-        <f t="shared" si="20"/>
-        <v>20004</v>
+        <f t="shared" ref="A940:A989" si="21">A939+1</f>
+        <v>20002</v>
       </c>
       <c r="B940" s="14" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C940" s="14" t="s">
-        <v>2113</v>
+        <v>1969</v>
       </c>
       <c r="D940" s="14" t="s">
-        <v>2116</v>
+        <v>1972</v>
       </c>
       <c r="E940" s="14" t="s">
         <v>2090</v>
       </c>
-      <c r="F940" s="14"/>
-      <c r="G940" s="14"/>
-      <c r="H940" s="14"/>
-      <c r="I940" s="14"/>
-      <c r="J940" s="14"/>
-      <c r="K940" s="14"/>
+      <c r="F940" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G940" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H940" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I940" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="J940" s="14" t="s">
+        <v>1964</v>
+      </c>
+      <c r="K940" s="14" t="s">
+        <v>1947</v>
+      </c>
       <c r="L940" s="14"/>
       <c r="M940" s="14"/>
       <c r="N940" s="14"/>
@@ -47039,33 +47064,45 @@
       <c r="Q940" s="14"/>
       <c r="R940" s="14"/>
       <c r="S940" s="14" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="T940" s="14"/>
     </row>
     <row r="941" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A941" s="14">
-        <f t="shared" si="20"/>
-        <v>20005</v>
+        <f t="shared" si="21"/>
+        <v>20003</v>
       </c>
       <c r="B941" s="14" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C941" s="14" t="s">
-        <v>2114</v>
+        <v>1970</v>
       </c>
       <c r="D941" s="14" t="s">
-        <v>2117</v>
+        <v>1973</v>
       </c>
       <c r="E941" s="14" t="s">
         <v>2090</v>
       </c>
-      <c r="F941" s="14"/>
-      <c r="G941" s="14"/>
-      <c r="H941" s="14"/>
-      <c r="I941" s="14"/>
-      <c r="J941" s="14"/>
-      <c r="K941" s="14"/>
+      <c r="F941" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G941" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H941" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I941" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="J941" s="14" t="s">
+        <v>1964</v>
+      </c>
+      <c r="K941" s="14" t="s">
+        <v>1947</v>
+      </c>
       <c r="L941" s="14"/>
       <c r="M941" s="14"/>
       <c r="N941" s="14"/>
@@ -47074,23 +47111,23 @@
       <c r="Q941" s="14"/>
       <c r="R941" s="14"/>
       <c r="S941" s="14" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="T941" s="14"/>
     </row>
     <row r="942" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A942" s="14">
-        <f t="shared" si="20"/>
-        <v>20006</v>
+        <f t="shared" si="21"/>
+        <v>20004</v>
       </c>
       <c r="B942" s="14" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C942" s="14" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
       <c r="D942" s="14" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
       <c r="E942" s="14" t="s">
         <v>2090</v>
@@ -47109,23 +47146,27 @@
       <c r="Q942" s="14"/>
       <c r="R942" s="14"/>
       <c r="S942" s="14" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="T942" s="14"/>
     </row>
     <row r="943" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A943" s="14">
-        <f t="shared" si="20"/>
-        <v>20007</v>
+        <f t="shared" si="21"/>
+        <v>20005</v>
       </c>
       <c r="B943" s="14" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C943" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="D943" s="14"/>
-      <c r="E943" s="14"/>
+        <v>2114</v>
+      </c>
+      <c r="D943" s="14" t="s">
+        <v>2117</v>
+      </c>
+      <c r="E943" s="14" t="s">
+        <v>2090</v>
+      </c>
       <c r="F943" s="14"/>
       <c r="G943" s="14"/>
       <c r="H943" s="14"/>
@@ -47140,21 +47181,27 @@
       <c r="Q943" s="14"/>
       <c r="R943" s="14"/>
       <c r="S943" s="14" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="T943" s="14"/>
     </row>
     <row r="944" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A944" s="14">
-        <f t="shared" si="20"/>
-        <v>20008</v>
+        <f t="shared" si="21"/>
+        <v>20006</v>
       </c>
       <c r="B944" s="14" t="s">
-        <v>598</v>
-      </c>
-      <c r="C944" s="14"/>
-      <c r="D944" s="14"/>
-      <c r="E944" s="14"/>
+        <v>605</v>
+      </c>
+      <c r="C944" s="14" t="s">
+        <v>2115</v>
+      </c>
+      <c r="D944" s="14" t="s">
+        <v>2118</v>
+      </c>
+      <c r="E944" s="14" t="s">
+        <v>2090</v>
+      </c>
       <c r="F944" s="14"/>
       <c r="G944" s="14"/>
       <c r="H944" s="14"/>
@@ -47169,19 +47216,21 @@
       <c r="Q944" s="14"/>
       <c r="R944" s="14"/>
       <c r="S944" s="14" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="T944" s="14"/>
     </row>
     <row r="945" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A945" s="14">
-        <f t="shared" si="20"/>
-        <v>20009</v>
+        <f t="shared" si="21"/>
+        <v>20007</v>
       </c>
       <c r="B945" s="14" t="s">
-        <v>608</v>
-      </c>
-      <c r="C945" s="14"/>
+        <v>607</v>
+      </c>
+      <c r="C945" s="14" t="s">
+        <v>346</v>
+      </c>
       <c r="D945" s="14"/>
       <c r="E945" s="14"/>
       <c r="F945" s="14"/>
@@ -47198,17 +47247,17 @@
       <c r="Q945" s="14"/>
       <c r="R945" s="14"/>
       <c r="S945" s="14" t="s">
-        <v>904</v>
+        <v>1152</v>
       </c>
       <c r="T945" s="14"/>
     </row>
     <row r="946" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A946" s="14">
-        <f t="shared" si="20"/>
-        <v>20010</v>
+        <f t="shared" si="21"/>
+        <v>20008</v>
       </c>
       <c r="B946" s="14" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="C946" s="14"/>
       <c r="D946" s="14"/>
@@ -47227,17 +47276,17 @@
       <c r="Q946" s="14"/>
       <c r="R946" s="14"/>
       <c r="S946" s="14" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="T946" s="14"/>
     </row>
     <row r="947" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A947" s="14">
-        <f t="shared" si="20"/>
-        <v>20011</v>
+        <f t="shared" si="21"/>
+        <v>20009</v>
       </c>
       <c r="B947" s="14" t="s">
-        <v>1893</v>
+        <v>608</v>
       </c>
       <c r="C947" s="14"/>
       <c r="D947" s="14"/>
@@ -47256,17 +47305,17 @@
       <c r="Q947" s="14"/>
       <c r="R947" s="14"/>
       <c r="S947" s="14" t="s">
-        <v>1155</v>
+        <v>904</v>
       </c>
       <c r="T947" s="14"/>
     </row>
     <row r="948" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A948" s="14">
-        <f t="shared" si="20"/>
-        <v>20012</v>
+        <f t="shared" si="21"/>
+        <v>20010</v>
       </c>
       <c r="B948" s="14" t="s">
-        <v>1894</v>
+        <v>609</v>
       </c>
       <c r="C948" s="14"/>
       <c r="D948" s="14"/>
@@ -47285,17 +47334,17 @@
       <c r="Q948" s="14"/>
       <c r="R948" s="14"/>
       <c r="S948" s="14" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="T948" s="14"/>
     </row>
     <row r="949" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A949" s="14">
-        <f t="shared" si="20"/>
-        <v>20013</v>
+        <f t="shared" si="21"/>
+        <v>20011</v>
       </c>
       <c r="B949" s="14" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
       <c r="C949" s="14"/>
       <c r="D949" s="14"/>
@@ -47314,17 +47363,17 @@
       <c r="Q949" s="14"/>
       <c r="R949" s="14"/>
       <c r="S949" s="14" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="T949" s="14"/>
     </row>
     <row r="950" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A950" s="14">
-        <f t="shared" si="20"/>
-        <v>20014</v>
+        <f t="shared" si="21"/>
+        <v>20012</v>
       </c>
       <c r="B950" s="14" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
       <c r="C950" s="14"/>
       <c r="D950" s="14"/>
@@ -47343,17 +47392,17 @@
       <c r="Q950" s="14"/>
       <c r="R950" s="14"/>
       <c r="S950" s="14" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="T950" s="14"/>
     </row>
     <row r="951" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A951" s="14">
-        <f t="shared" si="20"/>
-        <v>20015</v>
+        <f t="shared" si="21"/>
+        <v>20013</v>
       </c>
       <c r="B951" s="14" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
       <c r="C951" s="14"/>
       <c r="D951" s="14"/>
@@ -47372,17 +47421,17 @@
       <c r="Q951" s="14"/>
       <c r="R951" s="14"/>
       <c r="S951" s="14" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="T951" s="14"/>
     </row>
     <row r="952" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A952" s="14">
-        <f t="shared" si="20"/>
-        <v>20016</v>
+        <f t="shared" si="21"/>
+        <v>20014</v>
       </c>
       <c r="B952" s="14" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
       <c r="C952" s="14"/>
       <c r="D952" s="14"/>
@@ -47401,17 +47450,17 @@
       <c r="Q952" s="14"/>
       <c r="R952" s="14"/>
       <c r="S952" s="14" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="T952" s="14"/>
     </row>
     <row r="953" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A953" s="14">
-        <f t="shared" si="20"/>
-        <v>20017</v>
+        <f t="shared" si="21"/>
+        <v>20015</v>
       </c>
       <c r="B953" s="14" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
       <c r="C953" s="14"/>
       <c r="D953" s="14"/>
@@ -47430,17 +47479,17 @@
       <c r="Q953" s="14"/>
       <c r="R953" s="14"/>
       <c r="S953" s="14" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="T953" s="14"/>
     </row>
     <row r="954" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A954" s="14">
-        <f t="shared" si="20"/>
-        <v>20018</v>
+        <f t="shared" si="21"/>
+        <v>20016</v>
       </c>
       <c r="B954" s="14" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
       <c r="C954" s="14"/>
       <c r="D954" s="14"/>
@@ -47459,17 +47508,17 @@
       <c r="Q954" s="14"/>
       <c r="R954" s="14"/>
       <c r="S954" s="14" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="T954" s="14"/>
     </row>
     <row r="955" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A955" s="14">
-        <f t="shared" si="20"/>
-        <v>20019</v>
+        <f t="shared" si="21"/>
+        <v>20017</v>
       </c>
       <c r="B955" s="14" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
       <c r="C955" s="14"/>
       <c r="D955" s="14"/>
@@ -47488,17 +47537,17 @@
       <c r="Q955" s="14"/>
       <c r="R955" s="14"/>
       <c r="S955" s="14" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="T955" s="14"/>
     </row>
     <row r="956" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A956" s="14">
-        <f t="shared" si="20"/>
-        <v>20020</v>
+        <f t="shared" si="21"/>
+        <v>20018</v>
       </c>
       <c r="B956" s="14" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
       <c r="C956" s="14"/>
       <c r="D956" s="14"/>
@@ -47517,17 +47566,17 @@
       <c r="Q956" s="14"/>
       <c r="R956" s="14"/>
       <c r="S956" s="14" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="T956" s="14"/>
     </row>
     <row r="957" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A957" s="14">
-        <f t="shared" si="20"/>
-        <v>20021</v>
+        <f t="shared" si="21"/>
+        <v>20019</v>
       </c>
       <c r="B957" s="14" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="C957" s="14"/>
       <c r="D957" s="14"/>
@@ -47546,17 +47595,17 @@
       <c r="Q957" s="14"/>
       <c r="R957" s="14"/>
       <c r="S957" s="14" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="T957" s="14"/>
     </row>
     <row r="958" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A958" s="14">
-        <f t="shared" si="20"/>
-        <v>20022</v>
+        <f t="shared" si="21"/>
+        <v>20020</v>
       </c>
       <c r="B958" s="14" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
       <c r="C958" s="14"/>
       <c r="D958" s="14"/>
@@ -47575,17 +47624,17 @@
       <c r="Q958" s="14"/>
       <c r="R958" s="14"/>
       <c r="S958" s="14" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="T958" s="14"/>
     </row>
     <row r="959" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A959" s="14">
-        <f t="shared" si="20"/>
-        <v>20023</v>
+        <f t="shared" si="21"/>
+        <v>20021</v>
       </c>
       <c r="B959" s="14" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="C959" s="14"/>
       <c r="D959" s="14"/>
@@ -47604,17 +47653,17 @@
       <c r="Q959" s="14"/>
       <c r="R959" s="14"/>
       <c r="S959" s="14" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="T959" s="14"/>
     </row>
     <row r="960" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A960" s="14">
-        <f t="shared" si="20"/>
-        <v>20024</v>
+        <f t="shared" si="21"/>
+        <v>20022</v>
       </c>
       <c r="B960" s="14" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="C960" s="14"/>
       <c r="D960" s="14"/>
@@ -47633,17 +47682,17 @@
       <c r="Q960" s="14"/>
       <c r="R960" s="14"/>
       <c r="S960" s="14" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="T960" s="14"/>
     </row>
     <row r="961" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A961" s="14">
-        <f t="shared" si="20"/>
-        <v>20025</v>
+        <f t="shared" si="21"/>
+        <v>20023</v>
       </c>
       <c r="B961" s="14" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="C961" s="14"/>
       <c r="D961" s="14"/>
@@ -47662,17 +47711,17 @@
       <c r="Q961" s="14"/>
       <c r="R961" s="14"/>
       <c r="S961" s="14" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="T961" s="14"/>
     </row>
     <row r="962" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A962" s="14">
-        <f t="shared" si="20"/>
-        <v>20026</v>
+        <f t="shared" si="21"/>
+        <v>20024</v>
       </c>
       <c r="B962" s="14" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="C962" s="14"/>
       <c r="D962" s="14"/>
@@ -47691,17 +47740,17 @@
       <c r="Q962" s="14"/>
       <c r="R962" s="14"/>
       <c r="S962" s="14" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="T962" s="14"/>
     </row>
     <row r="963" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A963" s="14">
-        <f t="shared" si="20"/>
-        <v>20027</v>
+        <f t="shared" si="21"/>
+        <v>20025</v>
       </c>
       <c r="B963" s="14" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
       <c r="C963" s="14"/>
       <c r="D963" s="14"/>
@@ -47720,17 +47769,17 @@
       <c r="Q963" s="14"/>
       <c r="R963" s="14"/>
       <c r="S963" s="14" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="T963" s="14"/>
     </row>
     <row r="964" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A964" s="14">
-        <f t="shared" si="20"/>
-        <v>20028</v>
+        <f t="shared" si="21"/>
+        <v>20026</v>
       </c>
       <c r="B964" s="14" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="C964" s="14"/>
       <c r="D964" s="14"/>
@@ -47749,17 +47798,17 @@
       <c r="Q964" s="14"/>
       <c r="R964" s="14"/>
       <c r="S964" s="14" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="T964" s="14"/>
     </row>
     <row r="965" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A965" s="14">
-        <f t="shared" si="20"/>
-        <v>20029</v>
+        <f t="shared" si="21"/>
+        <v>20027</v>
       </c>
       <c r="B965" s="14" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="C965" s="14"/>
       <c r="D965" s="14"/>
@@ -47778,17 +47827,17 @@
       <c r="Q965" s="14"/>
       <c r="R965" s="14"/>
       <c r="S965" s="14" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="T965" s="14"/>
     </row>
     <row r="966" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A966" s="14">
-        <f t="shared" si="20"/>
-        <v>20030</v>
+        <f t="shared" si="21"/>
+        <v>20028</v>
       </c>
       <c r="B966" s="14" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
       <c r="C966" s="14"/>
       <c r="D966" s="14"/>
@@ -47807,17 +47856,17 @@
       <c r="Q966" s="14"/>
       <c r="R966" s="14"/>
       <c r="S966" s="14" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="T966" s="14"/>
     </row>
     <row r="967" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A967" s="14">
-        <f t="shared" si="20"/>
-        <v>20031</v>
+        <f t="shared" si="21"/>
+        <v>20029</v>
       </c>
       <c r="B967" s="14" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
       <c r="C967" s="14"/>
       <c r="D967" s="14"/>
@@ -47836,17 +47885,17 @@
       <c r="Q967" s="14"/>
       <c r="R967" s="14"/>
       <c r="S967" s="14" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="T967" s="14"/>
     </row>
     <row r="968" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A968" s="14">
-        <f t="shared" si="20"/>
-        <v>20032</v>
+        <f t="shared" si="21"/>
+        <v>20030</v>
       </c>
       <c r="B968" s="14" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="C968" s="14"/>
       <c r="D968" s="14"/>
@@ -47865,17 +47914,17 @@
       <c r="Q968" s="14"/>
       <c r="R968" s="14"/>
       <c r="S968" s="14" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="T968" s="14"/>
     </row>
     <row r="969" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A969" s="14">
-        <f t="shared" si="20"/>
-        <v>20033</v>
+        <f t="shared" si="21"/>
+        <v>20031</v>
       </c>
       <c r="B969" s="14" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="C969" s="14"/>
       <c r="D969" s="14"/>
@@ -47900,11 +47949,11 @@
     </row>
     <row r="970" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A970" s="14">
-        <f t="shared" si="20"/>
-        <v>20034</v>
+        <f t="shared" si="21"/>
+        <v>20032</v>
       </c>
       <c r="B970" s="14" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="C970" s="14"/>
       <c r="D970" s="14"/>
@@ -47923,17 +47972,17 @@
       <c r="Q970" s="14"/>
       <c r="R970" s="14"/>
       <c r="S970" s="14" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="T970" s="14"/>
     </row>
     <row r="971" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A971" s="14">
-        <f t="shared" si="20"/>
-        <v>20035</v>
+        <f t="shared" si="21"/>
+        <v>20033</v>
       </c>
       <c r="B971" s="14" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="C971" s="14"/>
       <c r="D971" s="14"/>
@@ -47952,17 +48001,17 @@
       <c r="Q971" s="14"/>
       <c r="R971" s="14"/>
       <c r="S971" s="14" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="T971" s="14"/>
     </row>
     <row r="972" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A972" s="14">
-        <f t="shared" si="20"/>
-        <v>20036</v>
+        <f t="shared" si="21"/>
+        <v>20034</v>
       </c>
       <c r="B972" s="14" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="C972" s="14"/>
       <c r="D972" s="14"/>
@@ -47981,17 +48030,17 @@
       <c r="Q972" s="14"/>
       <c r="R972" s="14"/>
       <c r="S972" s="14" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="T972" s="14"/>
     </row>
     <row r="973" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A973" s="14">
-        <f t="shared" si="20"/>
-        <v>20037</v>
+        <f t="shared" si="21"/>
+        <v>20035</v>
       </c>
       <c r="B973" s="14" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="C973" s="14"/>
       <c r="D973" s="14"/>
@@ -48010,17 +48059,17 @@
       <c r="Q973" s="14"/>
       <c r="R973" s="14"/>
       <c r="S973" s="14" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="T973" s="14"/>
     </row>
     <row r="974" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A974" s="14">
-        <f t="shared" si="20"/>
-        <v>20038</v>
+        <f t="shared" si="21"/>
+        <v>20036</v>
       </c>
       <c r="B974" s="14" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="C974" s="14"/>
       <c r="D974" s="14"/>
@@ -48039,17 +48088,17 @@
       <c r="Q974" s="14"/>
       <c r="R974" s="14"/>
       <c r="S974" s="14" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="T974" s="14"/>
     </row>
     <row r="975" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A975" s="14">
-        <f t="shared" si="20"/>
-        <v>20039</v>
+        <f t="shared" si="21"/>
+        <v>20037</v>
       </c>
       <c r="B975" s="14" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="C975" s="14"/>
       <c r="D975" s="14"/>
@@ -48068,17 +48117,17 @@
       <c r="Q975" s="14"/>
       <c r="R975" s="14"/>
       <c r="S975" s="14" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="T975" s="14"/>
     </row>
     <row r="976" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A976" s="14">
-        <f t="shared" si="20"/>
-        <v>20040</v>
+        <f t="shared" si="21"/>
+        <v>20038</v>
       </c>
       <c r="B976" s="14" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="C976" s="14"/>
       <c r="D976" s="14"/>
@@ -48097,17 +48146,17 @@
       <c r="Q976" s="14"/>
       <c r="R976" s="14"/>
       <c r="S976" s="14" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="T976" s="14"/>
     </row>
     <row r="977" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A977" s="14">
-        <f t="shared" si="20"/>
-        <v>20041</v>
+        <f t="shared" si="21"/>
+        <v>20039</v>
       </c>
       <c r="B977" s="14" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="C977" s="14"/>
       <c r="D977" s="14"/>
@@ -48126,17 +48175,17 @@
       <c r="Q977" s="14"/>
       <c r="R977" s="14"/>
       <c r="S977" s="14" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="T977" s="14"/>
     </row>
     <row r="978" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A978" s="14">
-        <f t="shared" si="20"/>
-        <v>20042</v>
+        <f t="shared" si="21"/>
+        <v>20040</v>
       </c>
       <c r="B978" s="14" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="C978" s="14"/>
       <c r="D978" s="14"/>
@@ -48155,17 +48204,17 @@
       <c r="Q978" s="14"/>
       <c r="R978" s="14"/>
       <c r="S978" s="14" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="T978" s="14"/>
     </row>
     <row r="979" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A979" s="14">
-        <f t="shared" si="20"/>
-        <v>20043</v>
+        <f t="shared" si="21"/>
+        <v>20041</v>
       </c>
       <c r="B979" s="14" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="C979" s="14"/>
       <c r="D979" s="14"/>
@@ -48190,11 +48239,11 @@
     </row>
     <row r="980" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A980" s="14">
-        <f t="shared" si="20"/>
-        <v>20044</v>
+        <f t="shared" si="21"/>
+        <v>20042</v>
       </c>
       <c r="B980" s="14" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="C980" s="14"/>
       <c r="D980" s="14"/>
@@ -48219,11 +48268,11 @@
     </row>
     <row r="981" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A981" s="14">
-        <f t="shared" si="20"/>
-        <v>20045</v>
+        <f t="shared" si="21"/>
+        <v>20043</v>
       </c>
       <c r="B981" s="14" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
       <c r="C981" s="14"/>
       <c r="D981" s="14"/>
@@ -48242,17 +48291,17 @@
       <c r="Q981" s="14"/>
       <c r="R981" s="14"/>
       <c r="S981" s="14" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="T981" s="14"/>
     </row>
     <row r="982" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A982" s="14">
-        <f t="shared" si="20"/>
-        <v>20046</v>
+        <f t="shared" si="21"/>
+        <v>20044</v>
       </c>
       <c r="B982" s="14" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="C982" s="14"/>
       <c r="D982" s="14"/>
@@ -48271,17 +48320,17 @@
       <c r="Q982" s="14"/>
       <c r="R982" s="14"/>
       <c r="S982" s="14" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="T982" s="14"/>
     </row>
     <row r="983" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A983" s="14">
-        <f t="shared" si="20"/>
-        <v>20047</v>
+        <f t="shared" si="21"/>
+        <v>20045</v>
       </c>
       <c r="B983" s="14" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
       <c r="C983" s="14"/>
       <c r="D983" s="14"/>
@@ -48300,17 +48349,17 @@
       <c r="Q983" s="14"/>
       <c r="R983" s="14"/>
       <c r="S983" s="14" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="T983" s="14"/>
     </row>
     <row r="984" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A984" s="14">
-        <f t="shared" si="20"/>
-        <v>20048</v>
+        <f t="shared" si="21"/>
+        <v>20046</v>
       </c>
       <c r="B984" s="14" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="C984" s="14"/>
       <c r="D984" s="14"/>
@@ -48329,17 +48378,17 @@
       <c r="Q984" s="14"/>
       <c r="R984" s="14"/>
       <c r="S984" s="14" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="T984" s="14"/>
     </row>
     <row r="985" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A985" s="14">
-        <f t="shared" si="20"/>
-        <v>20049</v>
+        <f t="shared" si="21"/>
+        <v>20047</v>
       </c>
       <c r="B985" s="14" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="C985" s="14"/>
       <c r="D985" s="14"/>
@@ -48358,17 +48407,17 @@
       <c r="Q985" s="14"/>
       <c r="R985" s="14"/>
       <c r="S985" s="14" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="T985" s="14"/>
     </row>
     <row r="986" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A986" s="14">
-        <f t="shared" si="20"/>
-        <v>20050</v>
+        <f t="shared" si="21"/>
+        <v>20048</v>
       </c>
       <c r="B986" s="14" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="C986" s="14"/>
       <c r="D986" s="14"/>
@@ -48387,17 +48436,17 @@
       <c r="Q986" s="14"/>
       <c r="R986" s="14"/>
       <c r="S986" s="14" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="T986" s="14"/>
     </row>
     <row r="987" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A987" s="14">
-        <f t="shared" si="20"/>
-        <v>20051</v>
+        <f t="shared" si="21"/>
+        <v>20049</v>
       </c>
       <c r="B987" s="14" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="C987" s="14"/>
       <c r="D987" s="14"/>
@@ -48415,14 +48464,66 @@
       <c r="P987" s="14"/>
       <c r="Q987" s="14"/>
       <c r="R987" s="14"/>
-      <c r="S987" s="14"/>
+      <c r="S987" s="14" t="s">
+        <v>1190</v>
+      </c>
       <c r="T987" s="14"/>
     </row>
     <row r="988" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A988" s="17"/>
+      <c r="A988" s="14">
+        <f t="shared" si="21"/>
+        <v>20050</v>
+      </c>
+      <c r="B988" s="14" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C988" s="14"/>
+      <c r="D988" s="14"/>
+      <c r="E988" s="14"/>
+      <c r="F988" s="14"/>
+      <c r="G988" s="14"/>
+      <c r="H988" s="14"/>
+      <c r="I988" s="14"/>
+      <c r="J988" s="14"/>
+      <c r="K988" s="14"/>
+      <c r="L988" s="14"/>
+      <c r="M988" s="14"/>
+      <c r="N988" s="14"/>
+      <c r="O988" s="14"/>
+      <c r="P988" s="14"/>
+      <c r="Q988" s="14"/>
+      <c r="R988" s="14"/>
+      <c r="S988" s="14" t="s">
+        <v>1191</v>
+      </c>
+      <c r="T988" s="14"/>
     </row>
     <row r="989" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A989" s="17"/>
+      <c r="A989" s="14">
+        <f t="shared" si="21"/>
+        <v>20051</v>
+      </c>
+      <c r="B989" s="14" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C989" s="14"/>
+      <c r="D989" s="14"/>
+      <c r="E989" s="14"/>
+      <c r="F989" s="14"/>
+      <c r="G989" s="14"/>
+      <c r="H989" s="14"/>
+      <c r="I989" s="14"/>
+      <c r="J989" s="14"/>
+      <c r="K989" s="14"/>
+      <c r="L989" s="14"/>
+      <c r="M989" s="14"/>
+      <c r="N989" s="14"/>
+      <c r="O989" s="14"/>
+      <c r="P989" s="14"/>
+      <c r="Q989" s="14"/>
+      <c r="R989" s="14"/>
+      <c r="S989" s="14"/>
+      <c r="T989" s="14"/>
     </row>
     <row r="990" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A990" s="17"/>
@@ -48747,6 +48848,12 @@
     </row>
     <row r="1097" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1097" s="17"/>
+    </row>
+    <row r="1098" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1098" s="17"/>
+    </row>
+    <row r="1099" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1099" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>